<commit_message>
Updates for Lesson 16
</commit_message>
<xml_diff>
--- a/data/singer_heights.xlsx
+++ b/data/singer_heights.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Downloads\Temp data folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Documents\GitHub\M221R\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8249BF3-2512-4B3B-AB63-A240F41868AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5798C3-5330-4A9B-AB2D-2EAFE22331F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22725" yWindow="-3015" windowWidth="14400" windowHeight="7365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="5">
-  <si>
-    <t>#NULL!</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>soprano</t>
   </si>
@@ -425,24 +422,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -735,9 +730,6 @@
       <c r="C22">
         <v>71</v>
       </c>
-      <c r="D22" t="s">
-        <v>0</v>
-      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
@@ -749,9 +741,6 @@
       <c r="C23">
         <v>70</v>
       </c>
-      <c r="D23" t="s">
-        <v>0</v>
-      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
@@ -762,9 +751,6 @@
       </c>
       <c r="C24">
         <v>74</v>
-      </c>
-      <c r="D24" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
@@ -777,9 +763,6 @@
       <c r="C25">
         <v>70</v>
       </c>
-      <c r="D25" t="s">
-        <v>0</v>
-      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
@@ -791,9 +774,6 @@
       <c r="C26">
         <v>75</v>
       </c>
-      <c r="D26" t="s">
-        <v>0</v>
-      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
@@ -805,9 +785,6 @@
       <c r="C27">
         <v>75</v>
       </c>
-      <c r="D27" t="s">
-        <v>0</v>
-      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
@@ -818,9 +795,6 @@
       </c>
       <c r="C28">
         <v>69</v>
-      </c>
-      <c r="D28" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
@@ -833,9 +807,6 @@
       <c r="C29">
         <v>72</v>
       </c>
-      <c r="D29" t="s">
-        <v>0</v>
-      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
@@ -847,9 +818,6 @@
       <c r="C30">
         <v>71</v>
       </c>
-      <c r="D30" t="s">
-        <v>0</v>
-      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
@@ -861,9 +829,6 @@
       <c r="C31">
         <v>70</v>
       </c>
-      <c r="D31" t="s">
-        <v>0</v>
-      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
@@ -875,11 +840,8 @@
       <c r="C32">
         <v>71</v>
       </c>
-      <c r="D32" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>61</v>
       </c>
@@ -889,11 +851,8 @@
       <c r="C33">
         <v>68</v>
       </c>
-      <c r="D33" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>65</v>
       </c>
@@ -903,11 +862,8 @@
       <c r="C34">
         <v>70</v>
       </c>
-      <c r="D34" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>66</v>
       </c>
@@ -917,11 +873,8 @@
       <c r="C35">
         <v>75</v>
       </c>
-      <c r="D35" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>65</v>
       </c>
@@ -931,64 +884,28 @@
       <c r="C36">
         <v>72</v>
       </c>
-      <c r="D36" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>62</v>
       </c>
       <c r="B37">
         <v>66</v>
       </c>
-      <c r="C37" t="s">
-        <v>0</v>
-      </c>
-      <c r="D37" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>72</v>
       </c>
-      <c r="B38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" t="s">
-        <v>0</v>
-      </c>
-      <c r="D38" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>70</v>
       </c>
-      <c r="B39" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" t="s">
-        <v>0</v>
-      </c>
-      <c r="D39" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>69</v>
-      </c>
-      <c r="B40" t="s">
-        <v>0</v>
-      </c>
-      <c r="C40" t="s">
-        <v>0</v>
-      </c>
-      <c r="D40" t="s">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>